<commit_message>
update to overview and data update
</commit_message>
<xml_diff>
--- a/Shiny App/Data/short.xlsx
+++ b/Shiny App/Data/short.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ola\OneDrive - Universiteit Utrecht\Documents\GitHub\UU-DS-courses\Shiny App\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9B65AA-87C5-41F4-B795-9E739EC60C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89C2AC3-E126-4694-AFFC-B7E8E5F4C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1152" windowWidth="22800" windowHeight="5808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>Strong theoretical base of data science practice and ethics</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Networks</t>
   </si>
   <si>
-    <t>Unsupervised Machine  Learning</t>
-  </si>
-  <si>
     <t>UML</t>
   </si>
   <si>
@@ -223,6 +220,18 @@
   </si>
   <si>
     <t>Causal Inference</t>
+  </si>
+  <si>
+    <t>Unsupervised Machine Learning</t>
+  </si>
+  <si>
+    <t>Haskell</t>
+  </si>
+  <si>
+    <t>Visual Studio</t>
+  </si>
+  <si>
+    <t>VS</t>
   </si>
 </sst>
 </file>
@@ -262,7 +271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -582,10 +591,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -593,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -601,7 +610,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -609,7 +618,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -633,7 +642,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -646,250 +655,266 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
         <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
         <v>32</v>
-      </c>
-      <c r="B25" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
         <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
         <v>39</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s">
         <v>43</v>
-      </c>
-      <c r="B32" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>